<commit_message>
update check check_hscode, add print in request and change tempalte upload
</commit_message>
<xml_diff>
--- a/assets/documents/template/template.xlsx
+++ b/assets/documents/template/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SENTRAL\CRJ\crj-project\assets\documents\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8CBB08-34B8-48CE-89B7-5D39E8265478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE6BDEC-E5E8-4944-AB4A-67D02B2B6DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86308F1F-307F-4073-BC66-AA3790BD1CE4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Sample-specification</t>
+  </si>
+  <si>
+    <t>FOB Price</t>
+  </si>
+  <si>
+    <t>CIF Price</t>
   </si>
 </sst>
 </file>
@@ -122,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,6 +162,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -167,30 +186,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -510,52 +535,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F498A41-CE72-453A-B7DD-64E5A1A5038D}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="137.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.6">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6">
+    <row r="2" spans="1:7" ht="15.6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>7000000001</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update check_hscode quotations sales_order
</commit_message>
<xml_diff>
--- a/assets/documents/template/template.xlsx
+++ b/assets/documents/template/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SENTRAL\CRJ\crj-project\assets\documents\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8A1797-09AF-4616-AC44-A29AFADD222C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FFE421-14E4-4D3C-A891-604F0C5035B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{86308F1F-307F-4073-BC66-AA3790BD1CE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{86308F1F-307F-4073-BC66-AA3790BD1CE4}"/>
   </bookViews>
   <sheets>
     <sheet name="imp_hscode" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>7000.000.001</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>pcs</t>
   </si>
 </sst>
 </file>
@@ -536,23 +548,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F498A41-CE72-453A-B7DD-64E5A1A5038D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="1" customWidth="1"/>
+    <col min="4" max="7" width="23.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -565,14 +577,23 @@
       <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -585,20 +606,32 @@
       <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
         <v>180.93</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="9"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>